<commit_message>
Monday sprint 2 backlog
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint 2 backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint 2 backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="92">
   <si>
     <t>Sprint 2</t>
   </si>
@@ -118,28 +118,31 @@
     <t>Accepted?</t>
   </si>
   <si>
-    <t>#19 as a researcher I want to access my own experiments?</t>
-  </si>
-  <si>
-    <t>When researcher logs in they can see all of their questionnaires, as well as data about it</t>
+    <t>As a principal researcher, I want full access to my own experiments so that I can view and keep track of all the relevant data/progress at any time.</t>
+  </si>
+  <si>
+    <t>When researcher logs in they can see all of their questionnaires in one place, as well as data about it</t>
+  </si>
+  <si>
+    <t>NOT AN ACTIVE STORY UNLESS LATER WE NEED MORE VELOCITY</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>2. As a researcher, I want to be able to export data from the questionnaire so that the data can be used for analysis.</t>
+  </si>
+  <si>
+    <t>All of the questionairre responses can be downloaded in an accessible and easily processible format</t>
+  </si>
+  <si>
+    <t>Timothy, Laura</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>2. As a researcher, I want to be able to export data from the questionnaire so that the data can be used for analysis.</t>
-  </si>
-  <si>
-    <t>All of the questionairre responses can be downloaded in an accessible and easily processible format</t>
-  </si>
-  <si>
-    <t>Timothy, Laura</t>
-  </si>
-  <si>
-    <t>3. As a stakeholder, I want participants to only have access to questionnaires so that the rest of the experiment is private and safe</t>
-  </si>
-  <si>
-    <t>When participants log in, they will only have access to questionnaires on their homepage.</t>
+    <t>(removed story #9 as it is more of an acceptance test than an independant story)</t>
   </si>
   <si>
     <t>4. As a researcher I want to be able to send questionnaires for participants to fill in so I can collect data from users</t>
@@ -189,7 +192,7 @@
     <t>Definition of Done:</t>
   </si>
   <si>
-    <t>Developer Tasks</t>
+    <t>Developer Tasks (each story broken down to steps to identify tasks)</t>
   </si>
   <si>
     <t>Create login page</t>
@@ -317,7 +320,7 @@
     <t>Yesterday Progress</t>
   </si>
   <si>
-    <t>Issues</t>
+    <t>Issues/Impediments</t>
   </si>
   <si>
     <t>Today's Work Plan</t>
@@ -327,6 +330,18 @@
   </si>
   <si>
     <t>M,B,S,I</t>
+  </si>
+  <si>
+    <t>2M, 5.5B, 0.5S</t>
+  </si>
+  <si>
+    <t>Yesterday we planned this sprint</t>
+  </si>
+  <si>
+    <t>Not many yet! Possible internet issues</t>
+  </si>
+  <si>
+    <t>- Get sendquestionairre integrated                       - Get login page setup                              - Work on frontend questionairre builder                                                                 -SQL CSV transpose</t>
   </si>
   <si>
     <t xml:space="preserve">daily scrum shouldn't cover the technicalities of work, it should focus on the next steps and help keep things moving - technicalities can be done at other times aside from the scrum </t>
@@ -339,7 +354,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -370,6 +385,11 @@
     <font>
       <sz val="8.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFA712A7"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -411,8 +431,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor theme="6"/>
+        <fgColor rgb="FFFFE2F9"/>
+        <bgColor rgb="FFFFE2F9"/>
       </patternFill>
     </fill>
   </fills>
@@ -530,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -587,10 +607,7 @@
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -605,22 +622,10 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -630,16 +635,16 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -647,6 +652,12 @@
     </xf>
     <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1003,341 +1014,341 @@
       <c r="D13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="H13" s="23">
+      <c r="F13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="25">
         <v>3.0</v>
       </c>
-      <c r="I13" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="I14" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="27"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="29" t="s">
+      <c r="I17" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="H15" s="31">
-        <v>2.0</v>
-      </c>
-      <c r="I15" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="32"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="I16" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="27"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="26">
-        <v>3.0</v>
-      </c>
-      <c r="I17" s="26" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="18">
-      <c r="A18" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="34" t="s">
+      <c r="A18" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="34" t="s">
+      <c r="E18" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="F18" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
     </row>
     <row r="19">
       <c r="G19" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="37"/>
+      <c r="J19" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="38" t="s">
-        <v>45</v>
+      <c r="G20" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K20" s="7"/>
       <c r="L20" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R20" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="J21" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="L21" s="24" t="s">
         <v>54</v>
       </c>
+      <c r="L21" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="N21" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="R21" s="24" t="s">
         <v>56</v>
       </c>
+      <c r="R21" s="23" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="24" t="s">
-        <v>57</v>
+      <c r="A22" s="23" t="s">
+        <v>58</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
+        <v>59</v>
+      </c>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
     </row>
     <row r="23">
-      <c r="A23" s="24" t="s">
-        <v>59</v>
+      <c r="A23" s="23" t="s">
+        <v>60</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="J23" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="N23" s="24" t="s">
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="J23" s="23" t="s">
         <v>62</v>
       </c>
+      <c r="N23" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="P23" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="39" t="s">
-        <v>64</v>
+      <c r="A24" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="J24" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="N24" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="J24" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="P24" s="24" t="s">
+      <c r="N24" s="23" t="s">
         <v>67</v>
+      </c>
+      <c r="P24" s="23" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J25" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="P25" s="24" t="s">
+      <c r="J25" s="23" t="s">
         <v>71</v>
       </c>
+      <c r="P25" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="24" t="s">
-        <v>72</v>
+      <c r="A26" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30">
       <c r="I30" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="40" t="s">
-        <v>78</v>
+      <c r="A31" s="35" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="B32" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="41" t="s">
+      <c r="C32" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="F32" s="42"/>
-      <c r="G32" s="41" t="s">
+      <c r="D32" s="37"/>
+      <c r="E32" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="H32" s="43"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H32" s="38"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C33" s="7"/>
     </row>
     <row r="34">
-      <c r="A34" s="44"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="G34" s="24"/>
+      <c r="A34" s="39">
+        <v>44228.0</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="44"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="G35" s="45"/>
-      <c r="I35" s="46" t="s">
-        <v>86</v>
+      <c r="A35" s="41"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="G35" s="42"/>
+      <c r="I35" s="43" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="44"/>
-      <c r="C36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="G36" s="24"/>
+      <c r="A36" s="41"/>
+      <c r="C36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="G36" s="23"/>
     </row>
     <row r="37">
-      <c r="A37" s="44"/>
-      <c r="E37" s="24"/>
-      <c r="G37" s="24"/>
+      <c r="A37" s="41"/>
+      <c r="E37" s="23"/>
+      <c r="G37" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="79">
+  <mergeCells count="77">
     <mergeCell ref="J23:K23"/>
     <mergeCell ref="L23:M23"/>
     <mergeCell ref="N23:O23"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J19:K19"/>
     <mergeCell ref="G20:H22"/>
     <mergeCell ref="J21:K21"/>
     <mergeCell ref="L21:M21"/>
     <mergeCell ref="N21:O21"/>
+    <mergeCell ref="J19:N19"/>
     <mergeCell ref="P24:Q24"/>
     <mergeCell ref="R24:S24"/>
     <mergeCell ref="N25:O25"/>
@@ -1367,11 +1378,11 @@
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
     <mergeCell ref="I35:K38"/>
     <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:C12"/>
     <mergeCell ref="D11:E12"/>
@@ -1379,15 +1390,13 @@
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A15:K15"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="A16:C16"/>

</xml_diff>